<commit_message>
Xamarin project (Network_Lock) moved to 'Project_Mobile' folder Rust project (locker_pi) created in 'Project_Rust' folder
In locker_pi:
    beginning command line parsing and prgram execution
    helper modules: command_line.rs, time_window.rs, and debugging.rs
    brainstorming: notes.txt
</commit_message>
<xml_diff>
--- a/Sprint_Tracking.xlsx
+++ b/Sprint_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Russell\Desktop\CloneHome\seniorProject\LockerPi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFEEB62-8EFC-4B50-B2F8-6EA7BC4CCD1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB77CBF4-A55A-4164-9EDD-ECDCB083FD86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65A5ADA9-51E1-46B4-8EAF-425C26E1E83B}"/>
   </bookViews>
@@ -201,7 +201,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -401,15 +401,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -473,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -525,25 +516,24 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -860,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90464733-25E4-4107-B886-5827D3AF02FF}">
-  <dimension ref="B1:K47"/>
+  <dimension ref="B1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,11 +922,11 @@
       </c>
       <c r="J6" s="6">
         <f>SUM(E8:E47)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K6" s="7">
         <f>I6-J6</f>
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -948,16 +938,18 @@
       <c r="E7" s="17"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="22">
-        <v>1</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="25" t="str">
+      <c r="B8" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+      <c r="D8" s="25">
+        <v>43793</v>
+      </c>
+      <c r="E8" s="22">
         <f>IF(D8="","",C8)</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -967,10 +959,12 @@
       <c r="C9" s="16">
         <v>1</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17" t="str">
+      <c r="D9" s="18">
+        <v>43794</v>
+      </c>
+      <c r="E9" s="17">
         <f t="shared" ref="E9:E47" si="0">IF(D9="","",C9)</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -1117,14 +1111,14 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="23">
-        <v>1</v>
-      </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="27" t="str">
+      <c r="C21" s="20">
+        <v>1</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1150,14 +1144,14 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="19">
         <v>2</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="25" t="str">
+      <c r="D24" s="19"/>
+      <c r="E24" s="22" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1267,14 +1261,14 @@
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="23">
-        <v>1</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="27" t="str">
+      <c r="C33" s="20">
+        <v>1</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="24" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1289,12 +1283,12 @@
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="25" t="str">
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="22" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1332,10 +1326,12 @@
       <c r="C38" s="16">
         <v>1</v>
       </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="D38" s="18">
+        <v>43794</v>
+      </c>
+      <c r="E38" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
@@ -1358,23 +1354,27 @@
       <c r="C40" s="16">
         <v>1</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="D40" s="18">
+        <v>43794</v>
+      </c>
+      <c r="E40" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="23">
-        <v>1</v>
-      </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C41" s="20">
+        <v>1</v>
+      </c>
+      <c r="D41" s="26">
+        <v>43794</v>
+      </c>
+      <c r="E41" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -1387,12 +1387,12 @@
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="25" t="str">
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="22" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1436,16 +1436,63 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="19" t="s">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="20">
+      <c r="C47" s="16">
         <v>2</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="21" t="str">
-        <f t="shared" si="0"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="17" t="str">
+        <f t="shared" ref="E48:E52" si="1">IF(D48="","",C48)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="15"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="15"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="15"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="18">
+        <v>42129</v>
+      </c>
+      <c r="E51" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="15"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="17" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
updated Research/Notes.txt, updated Spring_Tracking.xlsx, added network scanner ipscan to find raspberry pi ip address if needed
</commit_message>
<xml_diff>
--- a/Sprint_Tracking.xlsx
+++ b/Sprint_Tracking.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Russell\Desktop\CloneHome\seniorProject\LockerPi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9D3004-F5D0-4C99-9740-AD68ACB52AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C88A63D-35AB-46EE-A190-753AE3457386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8910" yWindow="2115" windowWidth="15195" windowHeight="9360" activeTab="1" xr2:uid="{65A5ADA9-51E1-46B4-8EAF-425C26E1E83B}"/>
+    <workbookView xWindow="0" yWindow="2115" windowWidth="15195" windowHeight="9360" activeTab="1" xr2:uid="{65A5ADA9-51E1-46B4-8EAF-425C26E1E83B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprint 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sprint 4" sheetId="3" r:id="rId1"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Magnitude</t>
   </si>
@@ -225,6 +228,12 @@
   </si>
   <si>
     <t>TCP protocol</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>Start Date</t>
   </si>
 </sst>
 </file>
@@ -4618,10 +4627,957 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04187502-ECAB-4D2B-A6C4-F071573FB03C}">
+  <dimension ref="A1:L78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="30" style="15" customWidth="1"/>
+    <col min="3" max="4" width="11.28515625" style="14" customWidth="1"/>
+    <col min="5" max="8" width="11" style="14" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="15"/>
+    <col min="10" max="10" width="11.42578125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="15"/>
+    <col min="12" max="12" width="11.140625" style="15" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43864</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3">
+        <v>43871</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="13"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="J5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="13"/>
+      <c r="J6" s="19">
+        <f>SUM(C8:C47)</f>
+        <v>14</v>
+      </c>
+      <c r="K6" s="20">
+        <f>SUM(F8:F47)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="21">
+        <f>J6-K6</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2" t="str">
+        <f>IF(E8="","",C8)</f>
+        <v/>
+      </c>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="10" t="str">
+        <f t="shared" ref="F9:F36" si="0">IF(E9="","",C9)</f>
+        <v/>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="10">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="10">
+        <v>2</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="10">
+        <v>2</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G34" s="13"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G35" s="13"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G36" s="13"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="2" t="str">
+        <f t="shared" ref="F38:F52" si="1">IF(E38="","",C38)</f>
+        <v/>
+      </c>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G42" s="13"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G44" s="13"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G45" s="13"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G46" s="13"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G47" s="13"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G48" s="13"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G49" s="13"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G50" s="13"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G51" s="13"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G52" s="13"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="13"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="22"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="22"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="22"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="22"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="22"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="22"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="22"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="22"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="22"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="22"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="22"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="22"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="22"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="22"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="22"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="22"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="22"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37332D7B-D2DE-4648-B627-48A4CFAA6C17}">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -5484,7 +6440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90464733-25E4-4107-B886-5827D3AF02FF}">
   <dimension ref="A1:EI78"/>
   <sheetViews>

</xml_diff>